<commit_message>
Fix: roles and colunm
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="127">
   <si>
     <t>name</t>
   </si>
@@ -25,7 +25,7 @@
     <t>trilha</t>
   </si>
   <si>
-    <t>cargo</t>
+    <t>UserRole</t>
   </si>
   <si>
     <t>password</t>
@@ -37,10 +37,10 @@
     <t>vitor.gabriel@rocketcorp.com</t>
   </si>
   <si>
-    <t>consultor</t>
-  </si>
-  <si>
-    <t>colaborador</t>
+    <t>BUSINESSMAN</t>
+  </si>
+  <si>
+    <t>EMPLOYER</t>
   </si>
   <si>
     <t>vitor.gabrielrocketcorp2024.1</t>
@@ -52,7 +52,7 @@
     <t>yuri.da@rocketcorp.com</t>
   </si>
   <si>
-    <t>gestor</t>
+    <t>LEADER</t>
   </si>
   <si>
     <t>yuri.darocketcorp2024.1</t>
@@ -64,7 +64,7 @@
     <t>valentina.martins@rocketcorp.com</t>
   </si>
   <si>
-    <t>design</t>
+    <t>DESIGNER</t>
   </si>
   <si>
     <t>valentina.martinsrocketcorp2024.1</t>
@@ -76,6 +76,9 @@
     <t>luiza.carvalho@rocketcorp.com</t>
   </si>
   <si>
+    <t>MANAGER</t>
+  </si>
+  <si>
     <t>luiza.carvalhorocketcorp2024.1</t>
   </si>
   <si>
@@ -94,7 +97,10 @@
     <t>levi.teixeira@rocketcorp.com</t>
   </si>
   <si>
-    <t>dev</t>
+    <t>DEVELOPER</t>
+  </si>
+  <si>
+    <t>MENTOR</t>
   </si>
   <si>
     <t>levi.teixeirarocketcorp2024.1</t>
@@ -106,6 +112,9 @@
     <t>laura.barros@rocketcorp.com</t>
   </si>
   <si>
+    <t>ARCHITECT</t>
+  </si>
+  <si>
     <t>laura.barrosrocketcorp2024.1</t>
   </si>
   <si>
@@ -140,9 +149,6 @@
   </si>
   <si>
     <t>samuel.jesus@rocketcorp.com</t>
-  </si>
-  <si>
-    <t>dev_backend</t>
   </si>
   <si>
     <t>samuel.jesusrocketcorp2024.1</t>
@@ -789,7 +795,7 @@
     <col min="5" max="5" style="4" width="45.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -806,7 +812,7 @@
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -823,7 +829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -865,21 +871,21 @@
         <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>16</v>
@@ -888,117 +894,117 @@
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="E8" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>7</v>
@@ -1007,32 +1013,32 @@
         <v>8</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>16</v>
@@ -1041,49 +1047,49 @@
         <v>8</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
       <c r="A16" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
       <c r="A17" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
       <c r="A18" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>16</v>
@@ -1092,15 +1098,15 @@
         <v>8</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
       <c r="A19" s="2" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>16</v>
@@ -1109,168 +1115,168 @@
         <v>12</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5">
       <c r="A20" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5">
       <c r="A21" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5">
       <c r="A22" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5">
       <c r="A23" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5">
       <c r="A24" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>7</v>
@@ -1279,177 +1285,177 @@
         <v>12</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="15.75">
       <c r="A34" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="15.75">
       <c r="A35" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="15.75">
       <c r="A36" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="15.75">
       <c r="A37" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="15.75">
       <c r="A38" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="15.75">
       <c r="A39" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="15.75">

</xml_diff>

<commit_message>
Fix: roles and colunm~
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -22,7 +22,7 @@
     <t>email</t>
   </si>
   <si>
-    <t>trilha</t>
+    <t>ProjectRole</t>
   </si>
   <si>
     <t>UserRole</t>
@@ -1356,7 +1356,7 @@
         <v>108</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="15.75">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="3" t="s">
         <v>109</v>
       </c>

</xml_diff>